<commit_message>
Version 05 | Added code for ETF comparison from Yesterday
</commit_message>
<xml_diff>
--- a/Old/PFFV ETF vs ICE.xlsx
+++ b/Old/PFFV ETF vs ICE.xlsx
@@ -97,12 +97,12 @@
     <t>US67058H4092</t>
   </si>
   <si>
+    <t>US46131B5066</t>
+  </si>
+  <si>
     <t>US0605055914</t>
   </si>
   <si>
-    <t>US46131B5066</t>
-  </si>
-  <si>
     <t>BMG8192H1557</t>
   </si>
   <si>
@@ -130,51 +130,51 @@
     <t>US95082P3038</t>
   </si>
   <si>
+    <t>US38144G8042</t>
+  </si>
+  <si>
+    <t>US6494452021</t>
+  </si>
+  <si>
+    <t>US6952632023</t>
+  </si>
+  <si>
+    <t>US7591EP5063</t>
+  </si>
+  <si>
+    <t>US8574778556</t>
+  </si>
+  <si>
+    <t>US4932677028</t>
+  </si>
+  <si>
+    <t>US7591EP7044</t>
+  </si>
+  <si>
+    <t>US12542R7044</t>
+  </si>
+  <si>
     <t>US61747S5047</t>
   </si>
   <si>
-    <t>US6494452021</t>
-  </si>
-  <si>
-    <t>US6952632023</t>
-  </si>
-  <si>
-    <t>US7591EP5063</t>
-  </si>
-  <si>
-    <t>US8574778556</t>
-  </si>
-  <si>
-    <t>US4932677028</t>
-  </si>
-  <si>
-    <t>US7591EP7044</t>
-  </si>
-  <si>
-    <t>US12542R7044</t>
+    <t>US64828T7063</t>
+  </si>
+  <si>
+    <t>US61761J4067</t>
+  </si>
+  <si>
+    <t>US61762V6065</t>
+  </si>
+  <si>
+    <t>US12542R5063</t>
+  </si>
+  <si>
+    <t>US9029731554</t>
   </si>
   <si>
     <t>US67059T2042</t>
   </si>
   <si>
-    <t>US61761J4067</t>
-  </si>
-  <si>
-    <t>US61762V6065</t>
-  </si>
-  <si>
-    <t>US64828T7063</t>
-  </si>
-  <si>
-    <t>US38144G8042</t>
-  </si>
-  <si>
-    <t>US9029731554</t>
-  </si>
-  <si>
-    <t>US12542R5063</t>
-  </si>
-  <si>
     <t>US0256765035</t>
   </si>
   <si>
@@ -193,49 +193,55 @@
     <t>US0158578080</t>
   </si>
   <si>
+    <t>US0357108705</t>
+  </si>
+  <si>
     <t>US64828T4094</t>
   </si>
   <si>
     <t>US16934Q5053</t>
   </si>
   <si>
+    <t>US38143Y6656</t>
+  </si>
+  <si>
+    <t>US0256766025</t>
+  </si>
+  <si>
     <t>US1746102045</t>
   </si>
   <si>
-    <t>US0256766025</t>
-  </si>
-  <si>
     <t>US9290892093</t>
   </si>
   <si>
     <t>US9576384062</t>
   </si>
   <si>
+    <t>US55261F8721</t>
+  </si>
+  <si>
     <t>US90187B5075</t>
   </si>
   <si>
-    <t>US55261F8721</t>
-  </si>
-  <si>
     <t>US90187B3096</t>
   </si>
   <si>
+    <t>US38148B1089</t>
+  </si>
+  <si>
+    <t>BMG0684D3054</t>
+  </si>
+  <si>
+    <t>US7593518027</t>
+  </si>
+  <si>
     <t>US00123Q8722</t>
   </si>
   <si>
-    <t>US0357108705</t>
-  </si>
-  <si>
-    <t>US38143Y6656</t>
-  </si>
-  <si>
-    <t>US7593518027</t>
-  </si>
-  <si>
-    <t>US38148B1089</t>
-  </si>
-  <si>
-    <t>BMG0684D3054</t>
+    <t>US0357108473</t>
+  </si>
+  <si>
+    <t>US04686J3095</t>
   </si>
   <si>
     <t>US64828T3005</t>
@@ -244,18 +250,12 @@
     <t>US4884013081</t>
   </si>
   <si>
+    <t>US58844R8842</t>
+  </si>
+  <si>
     <t>US00123Q8078</t>
   </si>
   <si>
-    <t>US58844R8842</t>
-  </si>
-  <si>
-    <t>US0357108473</t>
-  </si>
-  <si>
-    <t>US04686J3095</t>
-  </si>
-  <si>
     <t>US00123Q5009</t>
   </si>
   <si>
@@ -268,12 +268,12 @@
     <t>US00123Q8565</t>
   </si>
   <si>
+    <t>US0605051798</t>
+  </si>
+  <si>
     <t>US00123Q6098</t>
   </si>
   <si>
-    <t>US0605051798</t>
-  </si>
-  <si>
     <t>US0605055831</t>
   </si>
   <si>
@@ -337,12 +337,12 @@
     <t>NS.PRC</t>
   </si>
   <si>
+    <t>IVR.PRC</t>
+  </si>
+  <si>
     <t>BML.PRJ</t>
   </si>
   <si>
-    <t>IVR.PRC</t>
-  </si>
-  <si>
     <t>SPNT.PRB</t>
   </si>
   <si>
@@ -370,51 +370,51 @@
     <t>WCC.PRA</t>
   </si>
   <si>
+    <t>GS.PRD</t>
+  </si>
+  <si>
+    <t>NYCB.PRA</t>
+  </si>
+  <si>
+    <t>PACWP</t>
+  </si>
+  <si>
+    <t>RF.PRB</t>
+  </si>
+  <si>
+    <t>STT.PRG</t>
+  </si>
+  <si>
+    <t>KEY.PRI</t>
+  </si>
+  <si>
+    <t>RF.PRC</t>
+  </si>
+  <si>
+    <t>CHSCM</t>
+  </si>
+  <si>
     <t>MS.PRA</t>
   </si>
   <si>
-    <t>NYCB.PRA</t>
-  </si>
-  <si>
-    <t>PACWP</t>
-  </si>
-  <si>
-    <t>RF.PRB</t>
-  </si>
-  <si>
-    <t>STT.PRG</t>
-  </si>
-  <si>
-    <t>KEY.PRI</t>
-  </si>
-  <si>
-    <t>RF.PRC</t>
-  </si>
-  <si>
-    <t>CHSCM</t>
+    <t>RITM.PRD</t>
+  </si>
+  <si>
+    <t>MS.PRI</t>
+  </si>
+  <si>
+    <t>MS.PRK</t>
+  </si>
+  <si>
+    <t>CHSCN</t>
+  </si>
+  <si>
+    <t>USB.PRH</t>
   </si>
   <si>
     <t>NSS</t>
   </si>
   <si>
-    <t>MS.PRI</t>
-  </si>
-  <si>
-    <t>MS.PRK</t>
-  </si>
-  <si>
-    <t>RITM.PRD</t>
-  </si>
-  <si>
-    <t>GS.PRD</t>
-  </si>
-  <si>
-    <t>USB.PRH</t>
-  </si>
-  <si>
-    <t>CHSCN</t>
-  </si>
-  <si>
     <t>AEL.PRA</t>
   </si>
   <si>
@@ -433,49 +433,55 @@
     <t>AQNB</t>
   </si>
   <si>
+    <t>NLY.PRF</t>
+  </si>
+  <si>
     <t>RITM.PRB</t>
   </si>
   <si>
     <t>CIM.PRC</t>
   </si>
   <si>
+    <t>GS.PRA</t>
+  </si>
+  <si>
+    <t>AEL.PRB</t>
+  </si>
+  <si>
     <t>CFG.PRD</t>
   </si>
   <si>
-    <t>AEL.PRB</t>
-  </si>
-  <si>
     <t>VOYA.PRB</t>
   </si>
   <si>
     <t>WAL.PRA</t>
   </si>
   <si>
+    <t>MTB.PRH</t>
+  </si>
+  <si>
     <t>TWO.PRC</t>
   </si>
   <si>
-    <t>MTB.PRH</t>
-  </si>
-  <si>
     <t>TWO.PRB</t>
   </si>
   <si>
+    <t>GS.PRK</t>
+  </si>
+  <si>
+    <t>ATH.PRA</t>
+  </si>
+  <si>
+    <t>RZB</t>
+  </si>
+  <si>
     <t>AGNCP</t>
   </si>
   <si>
-    <t>NLY.PRF</t>
-  </si>
-  <si>
-    <t>GS.PRA</t>
-  </si>
-  <si>
-    <t>RZB</t>
-  </si>
-  <si>
-    <t>GS.PRK</t>
-  </si>
-  <si>
-    <t>ATH.PRA</t>
+    <t>NLY.PRI</t>
+  </si>
+  <si>
+    <t>ATH.PRC</t>
   </si>
   <si>
     <t>RITM.PRA</t>
@@ -484,18 +490,12 @@
     <t>KMPB</t>
   </si>
   <si>
+    <t>MBINM</t>
+  </si>
+  <si>
     <t>AGNCO</t>
   </si>
   <si>
-    <t>MBINM</t>
-  </si>
-  <si>
-    <t>NLY.PRI</t>
-  </si>
-  <si>
-    <t>ATH.PRC</t>
-  </si>
-  <si>
     <t>AGNCN</t>
   </si>
   <si>
@@ -508,10 +508,10 @@
     <t>AGNCL</t>
   </si>
   <si>
+    <t>MER.PRK</t>
+  </si>
+  <si>
     <t>AGNCM</t>
-  </si>
-  <si>
-    <t>MER.PRK</t>
   </si>
   <si>
     <t>BML.PRL</t>
@@ -919,7 +919,7 @@
         <v>87</v>
       </c>
       <c r="D2">
-        <v>24.21</v>
+        <v>24.2</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -945,19 +945,19 @@
         <v>88</v>
       </c>
       <c r="D3">
-        <v>25.904687</v>
+        <v>26.03</v>
       </c>
       <c r="E3">
-        <v>2.91267</v>
+        <v>2.8911</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <v>298725</v>
+        <v>295085</v>
       </c>
       <c r="H3" s="1">
-        <v>298725</v>
+        <v>295085</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -971,7 +971,7 @@
         <v>89</v>
       </c>
       <c r="D4">
-        <v>23.26</v>
+        <v>23.19</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -997,19 +997,19 @@
         <v>90</v>
       </c>
       <c r="D5">
-        <v>25.160331</v>
+        <v>25.34</v>
       </c>
       <c r="E5">
-        <v>2.13804</v>
+        <v>2.09693</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
       </c>
       <c r="G5" s="1">
-        <v>225766</v>
+        <v>219855</v>
       </c>
       <c r="H5" s="1">
-        <v>225766</v>
+        <v>219855</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -1023,7 +1023,7 @@
         <v>91</v>
       </c>
       <c r="D6">
-        <v>23.88</v>
+        <v>24.25</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1049,19 +1049,19 @@
         <v>92</v>
       </c>
       <c r="D7">
-        <v>23.15</v>
+        <v>23.22</v>
       </c>
       <c r="E7">
-        <v>1.5712</v>
+        <v>1.56464</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
       </c>
       <c r="G7" s="1">
-        <v>180318</v>
+        <v>179024</v>
       </c>
       <c r="H7" s="1">
-        <v>180318</v>
+        <v>179024</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -1075,19 +1075,19 @@
         <v>93</v>
       </c>
       <c r="D8">
-        <v>22.65</v>
+        <v>22.95</v>
       </c>
       <c r="E8">
-        <v>1.31516</v>
+        <v>1.31497</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <v>154266</v>
+        <v>152227</v>
       </c>
       <c r="H8" s="1">
-        <v>154266</v>
+        <v>152227</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1101,7 +1101,7 @@
         <v>94</v>
       </c>
       <c r="D9">
-        <v>18.98</v>
+        <v>19.71</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -1127,19 +1127,19 @@
         <v>95</v>
       </c>
       <c r="D10">
-        <v>20.89</v>
+        <v>20.91</v>
       </c>
       <c r="E10">
-        <v>0.8883</v>
+        <v>0.8827700000000001</v>
       </c>
       <c r="F10" s="1">
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>112974</v>
+        <v>112164</v>
       </c>
       <c r="H10" s="1">
-        <v>112974</v>
+        <v>112164</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1153,7 +1153,7 @@
         <v>96</v>
       </c>
       <c r="D11">
-        <v>22.63031</v>
+        <v>22.95</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1179,19 +1179,19 @@
         <v>97</v>
       </c>
       <c r="D12">
-        <v>20.53</v>
+        <v>20.77</v>
       </c>
       <c r="E12">
-        <v>0.83326</v>
+        <v>0.83696</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>107833</v>
+        <v>107060</v>
       </c>
       <c r="H12" s="1">
-        <v>107833</v>
+        <v>107060</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -1205,7 +1205,7 @@
         <v>98</v>
       </c>
       <c r="D13">
-        <v>17.2</v>
+        <v>17.16</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1231,7 +1231,7 @@
         <v>99</v>
       </c>
       <c r="D14">
-        <v>17.25</v>
+        <v>17.29</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1257,7 +1257,7 @@
         <v>100</v>
       </c>
       <c r="D15">
-        <v>21.55</v>
+        <v>21.7149</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1283,7 +1283,7 @@
         <v>101</v>
       </c>
       <c r="D16">
-        <v>21.22</v>
+        <v>21</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1309,7 +1309,7 @@
         <v>102</v>
       </c>
       <c r="D17">
-        <v>23.67</v>
+        <v>23.74</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1361,7 +1361,7 @@
         <v>104</v>
       </c>
       <c r="D19">
-        <v>20.48</v>
+        <v>20.52</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1387,7 +1387,7 @@
         <v>105</v>
       </c>
       <c r="D20">
-        <v>17.08</v>
+        <v>16.6625</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1413,24 +1413,24 @@
         <v>106</v>
       </c>
       <c r="D21">
-        <v>25.23</v>
+        <v>25.25</v>
       </c>
       <c r="E21">
-        <v>0.72526</v>
+        <v>0.72087</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
       <c r="G21" s="1">
-        <v>76372</v>
+        <v>75850</v>
       </c>
       <c r="H21" s="1">
-        <v>76372</v>
+        <v>75850</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="2">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
         <v>27</v>
@@ -1439,24 +1439,24 @@
         <v>107</v>
       </c>
       <c r="D22">
-        <v>20.98</v>
+        <v>18.705</v>
       </c>
       <c r="E22">
-        <v>0.5989</v>
+        <v>0</v>
       </c>
       <c r="F22" s="1">
-        <v>0</v>
+        <v>75661</v>
       </c>
       <c r="G22" s="1">
-        <v>75842</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1">
-        <v>75842</v>
+        <v>-75661</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="2">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="B23" t="s">
         <v>28</v>
@@ -1465,19 +1465,19 @@
         <v>108</v>
       </c>
       <c r="D23">
-        <v>18.7982</v>
+        <v>20.9</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>0.59234</v>
       </c>
       <c r="F23" s="1">
-        <v>75661</v>
+        <v>0</v>
       </c>
       <c r="G23" s="1">
-        <v>0</v>
+        <v>75298</v>
       </c>
       <c r="H23" s="1">
-        <v>-75661</v>
+        <v>75298</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1491,7 +1491,7 @@
         <v>109</v>
       </c>
       <c r="D24">
-        <v>21.81</v>
+        <v>22.03</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1517,7 +1517,7 @@
         <v>110</v>
       </c>
       <c r="D25">
-        <v>18.7</v>
+        <v>19.14</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1543,19 +1543,19 @@
         <v>111</v>
       </c>
       <c r="D26">
-        <v>22.35</v>
+        <v>22.56</v>
       </c>
       <c r="E26">
-        <v>0.55867</v>
+        <v>0.56006</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
       </c>
       <c r="G26" s="1">
-        <v>66410</v>
+        <v>65956</v>
       </c>
       <c r="H26" s="1">
-        <v>66410</v>
+        <v>65956</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1569,7 +1569,7 @@
         <v>112</v>
       </c>
       <c r="D27">
-        <v>18.03</v>
+        <v>19.22</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1595,19 +1595,19 @@
         <v>113</v>
       </c>
       <c r="D28">
-        <v>23.29</v>
+        <v>23.4</v>
       </c>
       <c r="E28">
-        <v>3.10491</v>
+        <v>3.09823</v>
       </c>
       <c r="F28" s="1">
         <v>306912</v>
       </c>
       <c r="G28" s="1">
-        <v>354192</v>
+        <v>351768</v>
       </c>
       <c r="H28" s="1">
-        <v>47280</v>
+        <v>44856</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1621,19 +1621,19 @@
         <v>114</v>
       </c>
       <c r="D29">
-        <v>60.44</v>
+        <v>60</v>
       </c>
       <c r="E29">
-        <v>1.00719</v>
+        <v>0.99302</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
       </c>
       <c r="G29" s="1">
-        <v>44274</v>
+        <v>43971</v>
       </c>
       <c r="H29" s="1">
-        <v>44274</v>
+        <v>43971</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1647,19 +1647,19 @@
         <v>115</v>
       </c>
       <c r="D30">
-        <v>21.77</v>
+        <v>22.06</v>
       </c>
       <c r="E30">
-        <v>2.1767</v>
+        <v>2.19061</v>
       </c>
       <c r="F30" s="1">
         <v>230344</v>
       </c>
       <c r="G30" s="1">
-        <v>265643</v>
+        <v>263827</v>
       </c>
       <c r="H30" s="1">
-        <v>35299</v>
+        <v>33483</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1673,19 +1673,19 @@
         <v>116</v>
       </c>
       <c r="D31">
-        <v>23.135</v>
+        <v>22.99</v>
       </c>
       <c r="E31">
-        <v>2.31318</v>
+        <v>2.28296</v>
       </c>
       <c r="F31" s="1">
         <v>230418</v>
       </c>
       <c r="G31" s="1">
-        <v>265643</v>
+        <v>263826</v>
       </c>
       <c r="H31" s="1">
-        <v>35225</v>
+        <v>33408</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1699,24 +1699,24 @@
         <v>117</v>
       </c>
       <c r="D32">
-        <v>26.72</v>
+        <v>26.58</v>
       </c>
       <c r="E32">
-        <v>2.40581</v>
+        <v>2.37683</v>
       </c>
       <c r="F32" s="1">
         <v>207471</v>
       </c>
       <c r="G32" s="1">
-        <v>239212</v>
+        <v>237576</v>
       </c>
       <c r="H32" s="1">
-        <v>31741</v>
+        <v>30105</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B33" t="s">
         <v>38</v>
@@ -1725,19 +1725,19 @@
         <v>118</v>
       </c>
       <c r="D33">
-        <v>19.936723</v>
+        <v>20.32</v>
       </c>
       <c r="E33">
-        <v>2.77382</v>
+        <v>3.69685</v>
       </c>
       <c r="F33" s="1">
-        <v>338033</v>
+        <v>512281</v>
       </c>
       <c r="G33" s="1">
-        <v>369644</v>
+        <v>483356</v>
       </c>
       <c r="H33" s="1">
-        <v>31611</v>
+        <v>-28925</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1751,19 +1751,19 @@
         <v>119</v>
       </c>
       <c r="D34">
-        <v>23</v>
+        <v>22.76</v>
       </c>
       <c r="E34">
-        <v>1.97389</v>
+        <v>1.93994</v>
       </c>
       <c r="F34" s="1">
         <v>197856</v>
       </c>
       <c r="G34" s="1">
-        <v>228010</v>
+        <v>226451</v>
       </c>
       <c r="H34" s="1">
-        <v>30154</v>
+        <v>28595</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1777,19 +1777,19 @@
         <v>120</v>
       </c>
       <c r="D35">
-        <v>14.5</v>
+        <v>15</v>
       </c>
       <c r="E35">
-        <v>1.24018</v>
+        <v>1.27417</v>
       </c>
       <c r="F35" s="1">
         <v>197176</v>
       </c>
       <c r="G35" s="1">
-        <v>227235</v>
+        <v>225681</v>
       </c>
       <c r="H35" s="1">
-        <v>30059</v>
+        <v>28505</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1803,19 +1803,19 @@
         <v>121</v>
       </c>
       <c r="D36">
-        <v>23.7</v>
+        <v>23.48</v>
       </c>
       <c r="E36">
-        <v>1.97473</v>
+        <v>1.94302</v>
       </c>
       <c r="F36" s="1">
         <v>192075</v>
       </c>
       <c r="G36" s="1">
-        <v>221370</v>
+        <v>219856</v>
       </c>
       <c r="H36" s="1">
-        <v>29295</v>
+        <v>27781</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1829,19 +1829,19 @@
         <v>122</v>
       </c>
       <c r="D37">
-        <v>25.01</v>
+        <v>24.92</v>
       </c>
       <c r="E37">
-        <v>2.08388</v>
+        <v>2.06218</v>
       </c>
       <c r="F37" s="1">
         <v>192078</v>
       </c>
       <c r="G37" s="1">
-        <v>221370</v>
+        <v>219856</v>
       </c>
       <c r="H37" s="1">
-        <v>29292</v>
+        <v>27778</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1855,19 +1855,19 @@
         <v>123</v>
       </c>
       <c r="D38">
-        <v>22.78</v>
+        <v>22.94</v>
       </c>
       <c r="E38">
-        <v>1.89807</v>
+        <v>1.89833</v>
       </c>
       <c r="F38" s="1">
         <v>192078</v>
       </c>
       <c r="G38" s="1">
-        <v>221369</v>
+        <v>219855</v>
       </c>
       <c r="H38" s="1">
-        <v>29291</v>
+        <v>27777</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1881,19 +1881,19 @@
         <v>124</v>
       </c>
       <c r="D39">
-        <v>21.43</v>
+        <v>21.1</v>
       </c>
       <c r="E39">
-        <v>1.78559</v>
+        <v>1.74607</v>
       </c>
       <c r="F39" s="1">
         <v>192105</v>
       </c>
       <c r="G39" s="1">
-        <v>221370</v>
+        <v>219856</v>
       </c>
       <c r="H39" s="1">
-        <v>29265</v>
+        <v>27751</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1907,24 +1907,24 @@
         <v>125</v>
       </c>
       <c r="D40">
-        <v>24.38</v>
+        <v>24.54</v>
       </c>
       <c r="E40">
-        <v>2.00092</v>
+        <v>2.00027</v>
       </c>
       <c r="F40" s="1">
         <v>189237</v>
       </c>
       <c r="G40" s="1">
-        <v>218049</v>
+        <v>216557</v>
       </c>
       <c r="H40" s="1">
-        <v>28812</v>
+        <v>27320</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" s="2">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
         <v>46</v>
@@ -1933,24 +1933,24 @@
         <v>126</v>
       </c>
       <c r="D41">
-        <v>24.607268</v>
+        <v>20.15</v>
       </c>
       <c r="E41">
-        <v>1.69899</v>
+        <v>2.76829</v>
       </c>
       <c r="F41" s="1">
-        <v>154824</v>
+        <v>338033</v>
       </c>
       <c r="G41" s="1">
-        <v>183437</v>
+        <v>365002</v>
       </c>
       <c r="H41" s="1">
-        <v>28613</v>
+        <v>26969</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" s="2">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B42" t="s">
         <v>47</v>
@@ -1959,24 +1959,24 @@
         <v>127</v>
       </c>
       <c r="D42">
-        <v>24.521562</v>
+        <v>19.45</v>
       </c>
       <c r="E42">
-        <v>3.09861</v>
+        <v>1.49686</v>
       </c>
       <c r="F42" s="1">
-        <v>307225</v>
+        <v>178874</v>
       </c>
       <c r="G42" s="1">
-        <v>335720</v>
+        <v>204466</v>
       </c>
       <c r="H42" s="1">
-        <v>28495</v>
+        <v>25592</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B43" t="s">
         <v>48</v>
@@ -1985,24 +1985,24 @@
         <v>128</v>
       </c>
       <c r="D43">
-        <v>24.254375</v>
+        <v>24.7</v>
       </c>
       <c r="E43">
-        <v>3.06131</v>
+        <v>3.0849</v>
       </c>
       <c r="F43" s="1">
-        <v>307241</v>
+        <v>307225</v>
       </c>
       <c r="G43" s="1">
-        <v>335333</v>
+        <v>331820</v>
       </c>
       <c r="H43" s="1">
-        <v>28092</v>
+        <v>24595</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
         <v>49</v>
@@ -2011,24 +2011,24 @@
         <v>129</v>
       </c>
       <c r="D44">
-        <v>18.75</v>
+        <v>24.5</v>
       </c>
       <c r="E44">
-        <v>1.45292</v>
+        <v>3.05992</v>
       </c>
       <c r="F44" s="1">
-        <v>178874</v>
+        <v>307241</v>
       </c>
       <c r="G44" s="1">
-        <v>205873</v>
+        <v>331820</v>
       </c>
       <c r="H44" s="1">
-        <v>26999</v>
+        <v>24579</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" s="2">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B45" t="s">
         <v>50</v>
@@ -2037,19 +2037,19 @@
         <v>130</v>
       </c>
       <c r="D45">
-        <v>20.12</v>
+        <v>24.51</v>
       </c>
       <c r="E45">
-        <v>3.68691</v>
+        <v>1.70929</v>
       </c>
       <c r="F45" s="1">
-        <v>512281</v>
+        <v>161478</v>
       </c>
       <c r="G45" s="1">
-        <v>486848</v>
+        <v>185281</v>
       </c>
       <c r="H45" s="1">
-        <v>-25433</v>
+        <v>23803</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2063,24 +2063,24 @@
         <v>131</v>
       </c>
       <c r="D46">
-        <v>18.680643</v>
+        <v>18.86</v>
       </c>
       <c r="E46">
-        <v>2.84799</v>
+        <v>2.85348</v>
       </c>
       <c r="F46" s="1">
         <v>379728</v>
       </c>
       <c r="G46" s="1">
-        <v>405047</v>
+        <v>401968</v>
       </c>
       <c r="H46" s="1">
-        <v>25319</v>
+        <v>22240</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" s="2">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B47" t="s">
         <v>52</v>
@@ -2089,19 +2089,19 @@
         <v>132</v>
       </c>
       <c r="D47">
-        <v>24.53</v>
+        <v>25.12</v>
       </c>
       <c r="E47">
-        <v>1.71966</v>
+        <v>1.67338</v>
       </c>
       <c r="F47" s="1">
-        <v>161478</v>
+        <v>154824</v>
       </c>
       <c r="G47" s="1">
-        <v>186253</v>
+        <v>176984</v>
       </c>
       <c r="H47" s="1">
-        <v>24775</v>
+        <v>22160</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2115,19 +2115,19 @@
         <v>133</v>
       </c>
       <c r="D48">
-        <v>22.04</v>
+        <v>22.372</v>
       </c>
       <c r="E48">
-        <v>1.46913</v>
+        <v>1.48106</v>
       </c>
       <c r="F48" s="1">
         <v>153904</v>
       </c>
       <c r="G48" s="1">
-        <v>177095</v>
+        <v>175884</v>
       </c>
       <c r="H48" s="1">
-        <v>23191</v>
+        <v>21980</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2141,19 +2141,19 @@
         <v>134</v>
       </c>
       <c r="D49">
-        <v>21.53</v>
+        <v>21.97</v>
       </c>
       <c r="E49">
-        <v>1.43514</v>
+        <v>1.45445</v>
       </c>
       <c r="F49" s="1">
         <v>153923</v>
       </c>
       <c r="G49" s="1">
-        <v>177096</v>
+        <v>175885</v>
       </c>
       <c r="H49" s="1">
-        <v>23173</v>
+        <v>21962</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2167,19 +2167,19 @@
         <v>135</v>
       </c>
       <c r="D50">
-        <v>17.45</v>
+        <v>18.36</v>
       </c>
       <c r="E50">
-        <v>1.15794</v>
+        <v>1.20999</v>
       </c>
       <c r="F50" s="1">
         <v>153364</v>
       </c>
       <c r="G50" s="1">
-        <v>176299</v>
+        <v>175093</v>
       </c>
       <c r="H50" s="1">
-        <v>22935</v>
+        <v>21729</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2193,19 +2193,19 @@
         <v>136</v>
       </c>
       <c r="D51">
-        <v>22.45</v>
+        <v>22.77</v>
       </c>
       <c r="E51">
-        <v>1.44034</v>
+        <v>1.45088</v>
       </c>
       <c r="F51" s="1">
         <v>148171</v>
       </c>
       <c r="G51" s="1">
-        <v>170454</v>
+        <v>169288</v>
       </c>
       <c r="H51" s="1">
-        <v>22283</v>
+        <v>21117</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2219,19 +2219,19 @@
         <v>137</v>
       </c>
       <c r="D52">
-        <v>21.065</v>
+        <v>20.86</v>
       </c>
       <c r="E52">
-        <v>1.22862</v>
+        <v>1.20834</v>
       </c>
       <c r="F52" s="1">
         <v>134751</v>
       </c>
       <c r="G52" s="1">
-        <v>154958</v>
+        <v>153898</v>
       </c>
       <c r="H52" s="1">
-        <v>20207</v>
+        <v>19147</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -2245,24 +2245,24 @@
         <v>138</v>
       </c>
       <c r="D53">
-        <v>23.29</v>
+        <v>23.2601</v>
       </c>
       <c r="E53">
-        <v>1.3584</v>
+        <v>1.34737</v>
       </c>
       <c r="F53" s="1">
         <v>134808</v>
       </c>
       <c r="G53" s="1">
-        <v>154959</v>
+        <v>153898</v>
       </c>
       <c r="H53" s="1">
-        <v>20151</v>
+        <v>19090</v>
       </c>
     </row>
     <row r="54" spans="1:8">
       <c r="A54" s="2">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B54" t="s">
         <v>59</v>
@@ -2271,24 +2271,24 @@
         <v>139</v>
       </c>
       <c r="D54">
-        <v>19.59</v>
+        <v>24.1415</v>
       </c>
       <c r="E54">
-        <v>0.9222399999999999</v>
+        <v>2.34336</v>
       </c>
       <c r="F54" s="1">
-        <v>106169</v>
+        <v>276284</v>
       </c>
       <c r="G54" s="1">
-        <v>125074</v>
+        <v>257889</v>
       </c>
       <c r="H54" s="1">
-        <v>18905</v>
+        <v>-18395</v>
       </c>
     </row>
     <row r="55" spans="1:8">
       <c r="A55" s="2">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B55" t="s">
         <v>60</v>
@@ -2297,24 +2297,24 @@
         <v>140</v>
       </c>
       <c r="D55">
-        <v>17.98</v>
+        <v>20.55</v>
       </c>
       <c r="E55">
-        <v>0.77903</v>
+        <v>0.9608100000000001</v>
       </c>
       <c r="F55" s="1">
-        <v>97418</v>
+        <v>106169</v>
       </c>
       <c r="G55" s="1">
-        <v>115113</v>
+        <v>124218</v>
       </c>
       <c r="H55" s="1">
-        <v>17695</v>
+        <v>18049</v>
       </c>
     </row>
     <row r="56" spans="1:8">
       <c r="A56" s="2">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>61</v>
@@ -2323,24 +2323,24 @@
         <v>141</v>
       </c>
       <c r="D56">
-        <v>23.5</v>
+        <v>18.16</v>
       </c>
       <c r="E56">
-        <v>1.17484</v>
+        <v>0.78144</v>
       </c>
       <c r="F56" s="1">
-        <v>115568</v>
+        <v>97418</v>
       </c>
       <c r="G56" s="1">
-        <v>132822</v>
+        <v>114324</v>
       </c>
       <c r="H56" s="1">
-        <v>17254</v>
+        <v>16906</v>
       </c>
     </row>
     <row r="57" spans="1:8">
       <c r="A57" s="2">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B57" t="s">
         <v>62</v>
@@ -2349,24 +2349,24 @@
         <v>142</v>
       </c>
       <c r="D57">
-        <v>24.19</v>
+        <v>20.11</v>
       </c>
       <c r="E57">
-        <v>1.20933</v>
+        <v>2.03258</v>
       </c>
       <c r="F57" s="1">
-        <v>115567</v>
+        <v>285059</v>
       </c>
       <c r="G57" s="1">
-        <v>132821</v>
+        <v>268531</v>
       </c>
       <c r="H57" s="1">
-        <v>17254</v>
+        <v>-16528</v>
       </c>
     </row>
     <row r="58" spans="1:8">
       <c r="A58" s="2">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B58" t="s">
         <v>63</v>
@@ -2375,24 +2375,24 @@
         <v>143</v>
       </c>
       <c r="D58">
-        <v>22.3</v>
+        <v>24.02</v>
       </c>
       <c r="E58">
-        <v>1.11485</v>
+        <v>1.19262</v>
       </c>
       <c r="F58" s="1">
-        <v>115579</v>
+        <v>115567</v>
       </c>
       <c r="G58" s="1">
-        <v>132822</v>
+        <v>131913</v>
       </c>
       <c r="H58" s="1">
-        <v>17243</v>
+        <v>16346</v>
       </c>
     </row>
     <row r="59" spans="1:8">
       <c r="A59" s="2">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="B59" t="s">
         <v>64</v>
@@ -2401,24 +2401,24 @@
         <v>144</v>
       </c>
       <c r="D59">
-        <v>13.09</v>
+        <v>23.58</v>
       </c>
       <c r="E59">
-        <v>0.65441</v>
+        <v>1.17077</v>
       </c>
       <c r="F59" s="1">
-        <v>115717</v>
+        <v>115568</v>
       </c>
       <c r="G59" s="1">
-        <v>132822</v>
+        <v>131913</v>
       </c>
       <c r="H59" s="1">
-        <v>17105</v>
+        <v>16345</v>
       </c>
     </row>
     <row r="60" spans="1:8">
       <c r="A60" s="2">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B60" t="s">
         <v>65</v>
@@ -2427,24 +2427,24 @@
         <v>145</v>
       </c>
       <c r="D60">
-        <v>18.87</v>
+        <v>22.39</v>
       </c>
       <c r="E60">
-        <v>0.92765</v>
+        <v>1.11169</v>
       </c>
       <c r="F60" s="1">
-        <v>113840</v>
+        <v>115579</v>
       </c>
       <c r="G60" s="1">
-        <v>130608</v>
+        <v>131913</v>
       </c>
       <c r="H60" s="1">
-        <v>16768</v>
+        <v>16334</v>
       </c>
     </row>
     <row r="61" spans="1:8">
       <c r="A61" s="2">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>66</v>
@@ -2453,24 +2453,24 @@
         <v>146</v>
       </c>
       <c r="D61">
-        <v>23.9</v>
+        <v>13.4</v>
       </c>
       <c r="E61">
-        <v>0.99569</v>
+        <v>0.66533</v>
       </c>
       <c r="F61" s="1">
-        <v>93921</v>
+        <v>115717</v>
       </c>
       <c r="G61" s="1">
-        <v>110684</v>
+        <v>131914</v>
       </c>
       <c r="H61" s="1">
-        <v>16763</v>
+        <v>16197</v>
       </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="2">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B62" t="s">
         <v>67</v>
@@ -2479,24 +2479,24 @@
         <v>147</v>
       </c>
       <c r="D62">
-        <v>18.9</v>
+        <v>24.59</v>
       </c>
       <c r="E62">
-        <v>0.9055</v>
+        <v>1.01743</v>
       </c>
       <c r="F62" s="1">
-        <v>110952</v>
+        <v>93921</v>
       </c>
       <c r="G62" s="1">
-        <v>127287</v>
+        <v>109927</v>
       </c>
       <c r="H62" s="1">
-        <v>16335</v>
+        <v>16006</v>
       </c>
     </row>
     <row r="63" spans="1:8">
       <c r="A63" s="2">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="B63" t="s">
         <v>68</v>
@@ -2505,24 +2505,24 @@
         <v>148</v>
       </c>
       <c r="D63">
-        <v>19.3371875</v>
+        <v>19.83</v>
       </c>
       <c r="E63">
-        <v>1.58107</v>
+        <v>0.96817</v>
       </c>
       <c r="F63" s="1">
-        <v>201883</v>
+        <v>113840</v>
       </c>
       <c r="G63" s="1">
-        <v>217228</v>
+        <v>129714</v>
       </c>
       <c r="H63" s="1">
-        <v>15345</v>
+        <v>15874</v>
       </c>
     </row>
     <row r="64" spans="1:8">
       <c r="A64" s="2">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B64" t="s">
         <v>69</v>
@@ -2531,24 +2531,24 @@
         <v>149</v>
       </c>
       <c r="D64">
-        <v>23.69</v>
+        <v>19.35</v>
       </c>
       <c r="E64">
-        <v>2.33034</v>
+        <v>0.92072</v>
       </c>
       <c r="F64" s="1">
-        <v>276284</v>
+        <v>110952</v>
       </c>
       <c r="G64" s="1">
-        <v>261344</v>
+        <v>126417</v>
       </c>
       <c r="H64" s="1">
-        <v>-14940</v>
+        <v>15465</v>
       </c>
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="2">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B65" t="s">
         <v>70</v>
@@ -2557,24 +2557,24 @@
         <v>150</v>
       </c>
       <c r="D65">
-        <v>20.4199</v>
+        <v>25.21</v>
       </c>
       <c r="E65">
-        <v>2.07881</v>
+        <v>2.37823</v>
       </c>
       <c r="F65" s="1">
-        <v>285059</v>
+        <v>265904</v>
       </c>
       <c r="G65" s="1">
-        <v>270471</v>
+        <v>250634</v>
       </c>
       <c r="H65" s="1">
-        <v>-14588</v>
+        <v>-15270</v>
       </c>
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="2">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B66" t="s">
         <v>71</v>
@@ -2583,24 +2583,24 @@
         <v>151</v>
       </c>
       <c r="D66">
-        <v>25.13</v>
+        <v>22.03</v>
       </c>
       <c r="E66">
-        <v>1.58733</v>
+        <v>2.56069</v>
       </c>
       <c r="F66" s="1">
-        <v>153839</v>
+        <v>324069</v>
       </c>
       <c r="G66" s="1">
-        <v>167816</v>
+        <v>308817</v>
       </c>
       <c r="H66" s="1">
-        <v>13977</v>
+        <v>-15252</v>
       </c>
     </row>
     <row r="67" spans="1:8">
       <c r="A67" s="2">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B67" t="s">
         <v>72</v>
@@ -2609,24 +2609,24 @@
         <v>152</v>
       </c>
       <c r="D67">
-        <v>25.16</v>
+        <v>25.35</v>
       </c>
       <c r="E67">
-        <v>2.39066</v>
+        <v>1.6089</v>
       </c>
       <c r="F67" s="1">
-        <v>265904</v>
+        <v>153839</v>
       </c>
       <c r="G67" s="1">
-        <v>252445</v>
+        <v>168620</v>
       </c>
       <c r="H67" s="1">
-        <v>-13459</v>
+        <v>14781</v>
       </c>
     </row>
     <row r="68" spans="1:8">
       <c r="A68" s="2">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B68" t="s">
         <v>73</v>
@@ -2635,24 +2635,24 @@
         <v>153</v>
       </c>
       <c r="D68">
-        <v>21.13</v>
+        <v>19.58</v>
       </c>
       <c r="E68">
-        <v>2.47382</v>
+        <v>1.58906</v>
       </c>
       <c r="F68" s="1">
-        <v>324069</v>
+        <v>201883</v>
       </c>
       <c r="G68" s="1">
-        <v>311048</v>
+        <v>215619</v>
       </c>
       <c r="H68" s="1">
-        <v>-13021</v>
+        <v>13736</v>
       </c>
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="2">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="B69" t="s">
         <v>74</v>
@@ -2661,24 +2661,24 @@
         <v>154</v>
       </c>
       <c r="D69">
-        <v>20.49</v>
+        <v>22.49</v>
       </c>
       <c r="E69">
-        <v>0.5301</v>
+        <v>1.34167</v>
       </c>
       <c r="F69" s="1">
-        <v>57516</v>
+        <v>170189</v>
       </c>
       <c r="G69" s="1">
-        <v>68734</v>
+        <v>158495</v>
       </c>
       <c r="H69" s="1">
-        <v>11218</v>
+        <v>-11694</v>
       </c>
     </row>
     <row r="70" spans="1:8">
       <c r="A70" s="2">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="B70" t="s">
         <v>75</v>
@@ -2687,24 +2687,24 @@
         <v>155</v>
       </c>
       <c r="D70">
-        <v>18.7</v>
+        <v>22.9</v>
       </c>
       <c r="E70">
-        <v>0.46744</v>
+        <v>1.85169</v>
       </c>
       <c r="F70" s="1">
-        <v>55552</v>
+        <v>225693</v>
       </c>
       <c r="G70" s="1">
-        <v>66411</v>
+        <v>214828</v>
       </c>
       <c r="H70" s="1">
-        <v>10859</v>
+        <v>-10865</v>
       </c>
     </row>
     <row r="71" spans="1:8">
       <c r="A71" s="2">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B71" t="s">
         <v>76</v>
@@ -2713,24 +2713,24 @@
         <v>156</v>
       </c>
       <c r="D71">
-        <v>20.53375</v>
+        <v>21.16</v>
       </c>
       <c r="E71">
-        <v>1.17225</v>
+        <v>0.5437</v>
       </c>
       <c r="F71" s="1">
-        <v>141553</v>
+        <v>57516</v>
       </c>
       <c r="G71" s="1">
-        <v>151674</v>
+        <v>68266</v>
       </c>
       <c r="H71" s="1">
-        <v>10121</v>
+        <v>10750</v>
       </c>
     </row>
     <row r="72" spans="1:8">
       <c r="A72" s="2">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B72" t="s">
         <v>77</v>
@@ -2739,24 +2739,24 @@
         <v>157</v>
       </c>
       <c r="D72">
-        <v>24.55</v>
+        <v>19</v>
       </c>
       <c r="E72">
-        <v>0.58013</v>
+        <v>0.47168</v>
       </c>
       <c r="F72" s="1">
-        <v>52961</v>
+        <v>55552</v>
       </c>
       <c r="G72" s="1">
-        <v>62782</v>
+        <v>65956</v>
       </c>
       <c r="H72" s="1">
-        <v>9821</v>
+        <v>10404</v>
       </c>
     </row>
     <row r="73" spans="1:8">
       <c r="A73" s="2">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="B73" t="s">
         <v>78</v>
@@ -2765,24 +2765,24 @@
         <v>158</v>
       </c>
       <c r="D73">
-        <v>22.405</v>
+        <v>25.02</v>
       </c>
       <c r="E73">
-        <v>1.3545</v>
+        <v>0.58819</v>
       </c>
       <c r="F73" s="1">
-        <v>170189</v>
+        <v>52961</v>
       </c>
       <c r="G73" s="1">
-        <v>160618</v>
+        <v>62458</v>
       </c>
       <c r="H73" s="1">
-        <v>-9571</v>
+        <v>9497</v>
       </c>
     </row>
     <row r="74" spans="1:8">
       <c r="A74" s="2">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B74" t="s">
         <v>79</v>
@@ -2791,19 +2791,19 @@
         <v>159</v>
       </c>
       <c r="D74">
-        <v>22.34</v>
+        <v>20.79</v>
       </c>
       <c r="E74">
-        <v>1.81946</v>
+        <v>1.18052</v>
       </c>
       <c r="F74" s="1">
-        <v>225693</v>
+        <v>141553</v>
       </c>
       <c r="G74" s="1">
-        <v>216381</v>
+        <v>150861</v>
       </c>
       <c r="H74" s="1">
-        <v>-9312</v>
+        <v>9308</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2817,19 +2817,19 @@
         <v>160</v>
       </c>
       <c r="D75">
-        <v>23.79871</v>
+        <v>23.93</v>
       </c>
       <c r="E75">
-        <v>1.10248</v>
+        <v>1.09817</v>
       </c>
       <c r="F75" s="1">
         <v>114369</v>
       </c>
       <c r="G75" s="1">
-        <v>123077</v>
+        <v>121923</v>
       </c>
       <c r="H75" s="1">
-        <v>8708</v>
+        <v>7554</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2846,16 +2846,16 @@
         <v>22.78</v>
       </c>
       <c r="E76">
-        <v>0.3906</v>
+        <v>0.39226</v>
       </c>
       <c r="F76" s="1">
         <v>38669</v>
       </c>
       <c r="G76" s="1">
-        <v>45555</v>
+        <v>45749</v>
       </c>
       <c r="H76" s="1">
-        <v>6886</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2869,19 +2869,19 @@
         <v>162</v>
       </c>
       <c r="D77">
-        <v>753.37582</v>
+        <v>757.55</v>
       </c>
       <c r="E77">
-        <v>1.65201</v>
+        <v>1.64652</v>
       </c>
       <c r="F77" s="1">
         <v>11872</v>
       </c>
       <c r="G77" s="1">
-        <v>5826</v>
+        <v>5775</v>
       </c>
       <c r="H77" s="1">
-        <v>-6046</v>
+        <v>-6097</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2895,24 +2895,24 @@
         <v>163</v>
       </c>
       <c r="D78">
-        <v>21.77562</v>
+        <v>21.54</v>
       </c>
       <c r="E78">
-        <v>0.46273</v>
+        <v>0.45561</v>
       </c>
       <c r="F78" s="1">
         <v>50591</v>
       </c>
       <c r="G78" s="1">
-        <v>56457</v>
+        <v>56196</v>
       </c>
       <c r="H78" s="1">
-        <v>5866</v>
+        <v>5605</v>
       </c>
     </row>
     <row r="79" spans="1:8">
       <c r="A79" s="2">
-        <v>56</v>
+        <v>1</v>
       </c>
       <c r="B79" t="s">
         <v>84</v>
@@ -2921,24 +2921,24 @@
         <v>164</v>
       </c>
       <c r="D79">
-        <v>20.4003125</v>
+        <v>25.09</v>
       </c>
       <c r="E79">
-        <v>0.68148</v>
+        <v>3.55036</v>
       </c>
       <c r="F79" s="1">
-        <v>83052</v>
+        <v>381354</v>
       </c>
       <c r="G79" s="1">
-        <v>88751</v>
+        <v>375950</v>
       </c>
       <c r="H79" s="1">
-        <v>5699</v>
+        <v>-5404</v>
       </c>
     </row>
     <row r="80" spans="1:8">
       <c r="A80" s="2">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="B80" t="s">
         <v>85</v>
@@ -2947,19 +2947,19 @@
         <v>165</v>
       </c>
       <c r="D80">
-        <v>25.1</v>
+        <v>20.46</v>
       </c>
       <c r="E80">
-        <v>3.57744</v>
+        <v>0.67664</v>
       </c>
       <c r="F80" s="1">
-        <v>381354</v>
+        <v>83052</v>
       </c>
       <c r="G80" s="1">
-        <v>378667</v>
+        <v>87864</v>
       </c>
       <c r="H80" s="1">
-        <v>-2687</v>
+        <v>4812</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2973,19 +2973,19 @@
         <v>166</v>
       </c>
       <c r="D81">
-        <v>20.24</v>
+        <v>20.25</v>
       </c>
       <c r="E81">
-        <v>1.14752</v>
+        <v>1.13985</v>
       </c>
       <c r="F81" s="1">
         <v>152332</v>
       </c>
       <c r="G81" s="1">
-        <v>150629</v>
+        <v>149548</v>
       </c>
       <c r="H81" s="1">
-        <v>-1703</v>
+        <v>-2784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>